<commit_message>
MATLAB script pulls & writes to correct directories
</commit_message>
<xml_diff>
--- a/datasheets/All names.xlsx
+++ b/datasheets/All names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinho\Documents\UIUC\ARCHES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD338FD0-9098-49A3-9474-04CB9987E37C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B97ECC5-073B-4D20-86C5-956E316BDD6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13764" yWindow="1488" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9648" yWindow="3732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C334"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="D231" sqref="D231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated All names to newest version
Adds more organization affiliations to investigators
</commit_message>
<xml_diff>
--- a/datasheets/All names.xlsx
+++ b/datasheets/All names.xlsx
@@ -1,43 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinho\Documents\UIUC\ARCHES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinho\Documents\UIUC\ARCHES\Github\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B97ECC5-073B-4D20-86C5-956E316BDD6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE978427-CC35-47DF-B358-3776ED8BD173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9648" yWindow="3732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$C$363</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$C$356</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="540">
   <si>
     <t>Name</t>
   </si>
@@ -1212,6 +1203,9 @@
     <t>Pavithra Rajeswaran</t>
   </si>
   <si>
+    <t>Pearl Richard H</t>
+  </si>
+  <si>
     <t>Richard.H.Pearl@osfhealthcare.org</t>
   </si>
   <si>
@@ -1233,9 +1227,6 @@
     <t>Qiong Wang</t>
   </si>
   <si>
-    <t>R.S. Sreenivas</t>
-  </si>
-  <si>
     <t>Rachel Lucas</t>
   </si>
   <si>
@@ -1254,24 +1245,15 @@
     <t>Rashid Bashir</t>
   </si>
   <si>
-    <t>Ravi Iyer</t>
-  </si>
-  <si>
     <t>Ravishankar Iyer</t>
   </si>
   <si>
     <t>Rayan Elkattah</t>
   </si>
   <si>
-    <t>Reddy</t>
-  </si>
-  <si>
     <t>Rhonda L. Johnson</t>
   </si>
   <si>
-    <t>Richar Sowers</t>
-  </si>
-  <si>
     <t>Richard Pearl</t>
   </si>
   <si>
@@ -1323,9 +1305,6 @@
     <t>Ryan Finkenbine</t>
   </si>
   <si>
-    <t>Ryan Reich</t>
-  </si>
-  <si>
     <t>Sandhya Pruthi</t>
   </si>
   <si>
@@ -1338,9 +1317,6 @@
     <t>Sanmi Koyejo</t>
   </si>
   <si>
-    <t>Sara Krzyzankiak</t>
-  </si>
-  <si>
     <t>Sara Moshage</t>
   </si>
   <si>
@@ -1539,10 +1515,139 @@
     <t>Zhi-Pei Liang</t>
   </si>
   <si>
+    <t>mkdasso2@illinois.edu</t>
+  </si>
+  <si>
+    <t>pferreir@illinois.edu</t>
+  </si>
+  <si>
+    <t>pramodch@illinois.edu</t>
+  </si>
+  <si>
+    <t>kumar1@illinois.edu</t>
+  </si>
+  <si>
+    <t>qwang04@illinois.edu</t>
+  </si>
+  <si>
+    <t>rsree@illinois.edu</t>
+  </si>
+  <si>
+    <t>rbashir@illinois.edu</t>
+  </si>
+  <si>
+    <t>rkiyer@illinois.edu</t>
+  </si>
+  <si>
+    <t>rayan.a.elkattah@osfhealthcare.org</t>
+  </si>
+  <si>
+    <t>chittaranjan.v.reddy@osfhealthcare.org</t>
+  </si>
+  <si>
+    <t>r-sowers@illinois.edu</t>
+  </si>
+  <si>
+    <t>rhpearl@uic.edu</t>
+  </si>
+  <si>
+    <t>tapping@uic.edu</t>
+  </si>
+  <si>
+    <t>riley.s.frenette@osfhealthcare.org</t>
+  </si>
+  <si>
+    <t>robert.r.riech@osfhealthcare.org</t>
+  </si>
+  <si>
+    <t>rxb@illinois.edu</t>
+  </si>
+  <si>
+    <t>croy@illinois.edu</t>
+  </si>
+  <si>
+    <t>roopa.foulger@osfhealthcare.org</t>
+  </si>
+  <si>
+    <t>rherna17@illinois.edu</t>
+  </si>
+  <si>
+    <t>dsouza@uwm.edu</t>
+  </si>
+  <si>
+    <t>girju@illinois.edu</t>
+  </si>
+  <si>
+    <t>rhc@illinois.edu</t>
+  </si>
+  <si>
+    <t>rubymen@illinois.edu</t>
+  </si>
+  <si>
+    <t>corey1@illinois.edu</t>
+  </si>
+  <si>
+    <t>ryanf@uic.edu</t>
+  </si>
+  <si>
+    <t>pruthi.sandhya@mayo.edu</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>sjp@illinois.edu</t>
+  </si>
+  <si>
+    <t>sjain1@illinois.edu</t>
+  </si>
+  <si>
+    <t>sanmi@illinois.edu</t>
+  </si>
+  <si>
+    <t>Sara Krzyzaniak</t>
+  </si>
+  <si>
+    <t>moshage1@illinois.edu</t>
+  </si>
+  <si>
+    <t>Sarah.A.StewartdeRamirez@osfhealthcare.org</t>
+  </si>
+  <si>
+    <t>sarah.n.zallek@ini.org</t>
+  </si>
+  <si>
+    <t>sasikanth.gorantla@osfhealthcare.org</t>
+  </si>
+  <si>
+    <t>scott.t.barrows@jumpsimulation.org</t>
+  </si>
+  <si>
+    <t>shannon.d.egli@jumpsimulation.org</t>
+  </si>
+  <si>
+    <t>stmejia@illinois.edu</t>
+  </si>
+  <si>
+    <t>sghosh9@illinois.edu</t>
+  </si>
+  <si>
+    <t>siddisu@uic.edu</t>
+  </si>
+  <si>
+    <t>stephanie.h.wieland@osfhealthcare.org</t>
+  </si>
+  <si>
+    <t>boppart@illinois.edu</t>
+  </si>
+  <si>
+    <t>lavalle@illinois.edu</t>
+  </si>
+  <si>
     <t>Joseph Irudayaraj</t>
   </si>
   <si>
-    <t>Richard H Pearl</t>
+    <t>Ryan Riech</t>
   </si>
 </sst>
 </file>
@@ -1917,10 +2022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C334"/>
+  <dimension ref="A1:C327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="D231" sqref="D231"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="C266" sqref="C266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3341,7 +3446,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>500</v>
+        <v>538</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>248</v>
@@ -3840,8 +3945,12 @@
       <c r="A188" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="B188" s="3"/>
-      <c r="C188" s="3"/>
+      <c r="B188" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
@@ -4184,10 +4293,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>501</v>
+        <v>391</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C222" t="s">
         <v>27</v>
@@ -4195,733 +4304,969 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+        <v>394</v>
+      </c>
+      <c r="B224" t="s">
+        <v>496</v>
+      </c>
+      <c r="C224" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+      <c r="C225" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+      <c r="B226" t="s">
+        <v>497</v>
+      </c>
+      <c r="C226" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+      <c r="B227" t="s">
+        <v>498</v>
+      </c>
+      <c r="C227" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+      <c r="B228" t="s">
+        <v>499</v>
+      </c>
+      <c r="C228" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+      <c r="B232" t="s">
+        <v>500</v>
+      </c>
+      <c r="C232" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+      <c r="B234" t="s">
+        <v>501</v>
+      </c>
+      <c r="C234" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+        <v>405</v>
+      </c>
+      <c r="B235" t="s">
+        <v>502</v>
+      </c>
+      <c r="C235" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+        <v>406</v>
+      </c>
+      <c r="B236" t="s">
+        <v>503</v>
+      </c>
+      <c r="C236" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="B237" t="s">
+        <v>504</v>
+      </c>
+      <c r="C237" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+      <c r="C238" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+        <v>408</v>
+      </c>
+      <c r="B239" t="s">
+        <v>506</v>
+      </c>
+      <c r="C239" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+        <v>409</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C240" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+      <c r="B241" t="s">
+        <v>507</v>
+      </c>
+      <c r="C241" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+      <c r="B242" t="s">
+        <v>506</v>
+      </c>
+      <c r="C242" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+      <c r="B243" t="s">
+        <v>508</v>
+      </c>
+      <c r="C243" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+      <c r="B244" t="s">
+        <v>509</v>
+      </c>
+      <c r="C244" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="C245" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+      <c r="B246" t="s">
+        <v>511</v>
+      </c>
+      <c r="C246" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+      <c r="B248" t="s">
+        <v>512</v>
+      </c>
+      <c r="C248" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+      <c r="B249" t="s">
+        <v>513</v>
+      </c>
+      <c r="C249" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+      <c r="B250" t="s">
+        <v>514</v>
+      </c>
+      <c r="C250" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+      <c r="B251" t="s">
+        <v>515</v>
+      </c>
+      <c r="C251" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+        <v>421</v>
+      </c>
+      <c r="B252" t="s">
+        <v>516</v>
+      </c>
+      <c r="C252" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+        <v>422</v>
+      </c>
+      <c r="B253" t="s">
+        <v>517</v>
+      </c>
+      <c r="C253" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+      <c r="B254" t="s">
+        <v>518</v>
+      </c>
+      <c r="C254" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+        <v>424</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C255" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+        <v>539</v>
+      </c>
+      <c r="B256" t="s">
+        <v>509</v>
+      </c>
+      <c r="C256" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B257" t="s">
+        <v>520</v>
+      </c>
+      <c r="C257" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B258" t="s">
+        <v>522</v>
+      </c>
+      <c r="C258" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B259" t="s">
+        <v>523</v>
+      </c>
+      <c r="C259" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B260" t="s">
+        <v>524</v>
+      </c>
+      <c r="C260" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
+        <v>525</v>
+      </c>
+      <c r="C261" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A262" t="s">
+      <c r="B262" t="s">
+        <v>526</v>
+      </c>
+      <c r="C262" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A263" t="s">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A264" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B264" t="s">
+        <v>527</v>
+      </c>
+      <c r="C264" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B265" t="s">
+        <v>528</v>
+      </c>
+      <c r="C265" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B266" t="s">
+        <v>529</v>
+      </c>
+      <c r="C266" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B267" t="s">
+        <v>530</v>
+      </c>
+      <c r="C267" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B268" t="s">
+        <v>531</v>
+      </c>
+      <c r="C268" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B269" t="s">
+        <v>532</v>
+      </c>
+      <c r="C269" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B270" t="s">
+        <v>533</v>
+      </c>
+      <c r="C270" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B271" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C271" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>439</v>
+      </c>
+      <c r="C272" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>440</v>
       </c>
+      <c r="C273" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>441</v>
       </c>
+      <c r="C274" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>442</v>
       </c>
+      <c r="B275" t="s">
+        <v>535</v>
+      </c>
+      <c r="C275" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>443</v>
       </c>
+      <c r="B276" t="s">
+        <v>536</v>
+      </c>
+      <c r="C276" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>443</v>
+        <v>444</v>
+      </c>
+      <c r="B277" t="s">
+        <v>537</v>
+      </c>
+      <c r="C277" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>444</v>
-      </c>
-      <c r="C278" t="s">
-        <v>7</v>
+        <v>445</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A328" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A329" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A330" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A331" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A332" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A333" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A334" t="s">
-        <v>499</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C363" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C356" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="mailto:arwool@illinois.edu" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{EA591B75-96D5-48FB-97BD-27FB1B3A8E5A}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{B507A6CB-6004-4507-94BE-03E6A2335B86}"/>
-    <hyperlink ref="B7" r:id="rId4" xr:uid="{7E519466-E73F-414C-8DE8-92DD98A87010}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{DBA4677E-94A7-4C9B-84D7-23ABB7D0AA2F}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{845DB7AE-38C9-44ED-A80C-810324EB3D23}"/>
-    <hyperlink ref="B11" r:id="rId7" xr:uid="{C8335C5A-1562-45F1-9F8E-905AB1EA3ABD}"/>
-    <hyperlink ref="B13" r:id="rId8" xr:uid="{5C4752E3-17FC-4B09-8F22-B69E731022E8}"/>
-    <hyperlink ref="B19" r:id="rId9" xr:uid="{CB3A86E7-85F7-46AA-B5B2-9BC889C0DE07}"/>
-    <hyperlink ref="B21" r:id="rId10" xr:uid="{159E0BFB-4908-4D16-A015-B72E21381A5A}"/>
-    <hyperlink ref="B22" r:id="rId11" xr:uid="{A5557EAD-7C9B-4DD9-90F3-EB9F15AED558}"/>
-    <hyperlink ref="B25" r:id="rId12" xr:uid="{6556F6E5-2571-4F49-BF21-47A8A2C19B88}"/>
-    <hyperlink ref="B26" r:id="rId13" xr:uid="{EC94D2A7-EABD-486B-AC42-8EFE8FB9EFF8}"/>
-    <hyperlink ref="B29" r:id="rId14" xr:uid="{F946018E-2FE1-40CD-AE07-4E08E74ED4BF}"/>
-    <hyperlink ref="B31" r:id="rId15" xr:uid="{69332BFE-C2E8-4F45-B8D4-4546E9ABFD32}"/>
-    <hyperlink ref="B32" r:id="rId16" xr:uid="{3AF4EE5D-DA70-4F08-B807-1521C9D480E1}"/>
-    <hyperlink ref="B33" r:id="rId17" xr:uid="{A152F1EF-B338-420F-8208-23707FE52480}"/>
-    <hyperlink ref="B34" r:id="rId18" xr:uid="{2F95BD72-02D9-4C45-A774-089CCB7AAC9F}"/>
-    <hyperlink ref="B36" r:id="rId19" xr:uid="{98271830-CFA9-4585-AAA6-A810FC2D8F3B}"/>
-    <hyperlink ref="B37" r:id="rId20" xr:uid="{8DC987F9-50B1-4182-AE90-45A851651C28}"/>
-    <hyperlink ref="B38" r:id="rId21" xr:uid="{C1F9A3EF-43DD-49DD-AF92-EBA5267153C3}"/>
-    <hyperlink ref="B39" r:id="rId22" xr:uid="{6A7F90F0-6039-4FE1-8596-E71AA80B22C8}"/>
-    <hyperlink ref="B40" r:id="rId23" xr:uid="{B259F1ED-5EC7-4A8E-92AB-99DFF589F389}"/>
-    <hyperlink ref="B41" r:id="rId24" xr:uid="{F081A824-B027-4356-AEE8-F699D46C008B}"/>
-    <hyperlink ref="B42" r:id="rId25" xr:uid="{882F5761-180E-4414-A754-081DE0BA7BAE}"/>
-    <hyperlink ref="B43" r:id="rId26" xr:uid="{26F0FEBE-21C1-475D-8BEE-608E21AA1444}"/>
-    <hyperlink ref="B44" r:id="rId27" xr:uid="{3D4C6C93-F5D5-4D9C-9112-2B2D361C952C}"/>
-    <hyperlink ref="B45" r:id="rId28" xr:uid="{15C7617E-3D2A-49CD-9A6E-1B725CC971A8}"/>
-    <hyperlink ref="B46" r:id="rId29" xr:uid="{2F58AB15-2CF0-4562-838D-43382DFDDE11}"/>
-    <hyperlink ref="B47" r:id="rId30" xr:uid="{18F582EF-1809-4B2E-85E1-4EBB6ECFA676}"/>
-    <hyperlink ref="B48" r:id="rId31" xr:uid="{4C815179-14D1-4772-9C2F-4CC71287AB0E}"/>
-    <hyperlink ref="B49" r:id="rId32" xr:uid="{19BA6B64-C6D4-4C2E-9853-FEFE1C3E43D5}"/>
-    <hyperlink ref="B50" r:id="rId33" xr:uid="{3BBD80AB-73F0-4704-A1C3-A061DF112423}"/>
-    <hyperlink ref="B51" r:id="rId34" xr:uid="{FDF55830-6958-4D7D-8AF3-00B930B9995B}"/>
-    <hyperlink ref="B52" r:id="rId35" xr:uid="{C1EEA9DB-7435-4CCD-A79C-8D496431D138}"/>
-    <hyperlink ref="B53" r:id="rId36" xr:uid="{66261464-D854-4008-83C7-9595794E8385}"/>
-    <hyperlink ref="B54" r:id="rId37" xr:uid="{AA389862-DD5F-4F66-B844-DBE525C2CF32}"/>
-    <hyperlink ref="B55" r:id="rId38" xr:uid="{223B3E7F-E5E2-43FA-B412-FC03CF526E3C}"/>
-    <hyperlink ref="B56" r:id="rId39" xr:uid="{B7CE26A6-2B2F-454E-BFE5-022322EF00DD}"/>
-    <hyperlink ref="B58" r:id="rId40" xr:uid="{779A80FA-C581-4388-B5FC-01DDF00C7298}"/>
-    <hyperlink ref="B59" r:id="rId41" xr:uid="{2B5D2C80-6043-42A7-92BF-8763E3A10665}"/>
-    <hyperlink ref="B62" r:id="rId42" xr:uid="{044007C3-52DA-4D8B-9C77-31DEEE16663C}"/>
-    <hyperlink ref="B64" r:id="rId43" xr:uid="{499363E0-857B-4AE5-B457-78DF195ADF78}"/>
-    <hyperlink ref="B65" r:id="rId44" xr:uid="{94620192-AE82-4B69-BA7F-E5E239BF691E}"/>
-    <hyperlink ref="B66" r:id="rId45" xr:uid="{E6BDD829-884D-42EC-BA0C-81F10C24BEAA}"/>
-    <hyperlink ref="B68" r:id="rId46" xr:uid="{CFDFB918-0D7B-456A-9452-FB8EC1CA3102}"/>
-    <hyperlink ref="B69" r:id="rId47" xr:uid="{75629B32-7781-423D-9C82-C8F75CA2BE63}"/>
-    <hyperlink ref="B70" r:id="rId48" xr:uid="{2504739A-A750-456A-BBB6-A8F99D6C6FBF}"/>
-    <hyperlink ref="B71" r:id="rId49" xr:uid="{49770369-BB92-44BC-B3EB-C61C681E0A06}"/>
-    <hyperlink ref="B72" r:id="rId50" xr:uid="{7F5CE8B2-97B9-424F-8021-C646736DE060}"/>
-    <hyperlink ref="B73" r:id="rId51" xr:uid="{419C7DFA-E63E-4348-BAF3-E150F81F9467}"/>
-    <hyperlink ref="B74" r:id="rId52" xr:uid="{F420F781-ED99-4A54-A25E-1C55CA0346F8}"/>
-    <hyperlink ref="B76" r:id="rId53" xr:uid="{AF2CAAAB-882D-4117-92BB-11F5F07B884A}"/>
-    <hyperlink ref="B79" r:id="rId54" xr:uid="{90C7CE80-8B25-4C03-958E-79E3AF81A647}"/>
-    <hyperlink ref="B80" r:id="rId55" xr:uid="{D8F6FF6C-C358-4A6A-949E-ED0C7D2F24A8}"/>
-    <hyperlink ref="B82" r:id="rId56" xr:uid="{28D51DE8-245A-4A78-8DDC-42B51DD22C30}"/>
-    <hyperlink ref="B83" r:id="rId57" xr:uid="{620FF6A8-B80D-4417-BFEB-DFB7796AA83E}"/>
-    <hyperlink ref="B85" r:id="rId58" xr:uid="{32A4E30B-5507-4E4F-8824-89341CA594BE}"/>
-    <hyperlink ref="B86" r:id="rId59" xr:uid="{EA97C198-1FF4-410D-856E-8E24366DD2FB}"/>
-    <hyperlink ref="B87" r:id="rId60" xr:uid="{CF450A80-874D-4A1F-8E44-1F643F80F219}"/>
-    <hyperlink ref="B88" r:id="rId61" xr:uid="{D5E03575-1485-4CB9-A283-0A7320AD3A64}"/>
-    <hyperlink ref="B89" r:id="rId62" xr:uid="{46137AEA-2F2A-44C7-8405-E406685EDD8B}"/>
-    <hyperlink ref="B90" r:id="rId63" xr:uid="{F190644C-3E11-4ECB-BC7E-5F349CE8F918}"/>
-    <hyperlink ref="B91" r:id="rId64" xr:uid="{9D629E81-E285-474D-B345-C3B1E2895B85}"/>
-    <hyperlink ref="B92" r:id="rId65" xr:uid="{5E9ED286-DAF6-4210-929A-3CB8E177185A}"/>
-    <hyperlink ref="B93" r:id="rId66" xr:uid="{3B77A403-0EE0-437E-A89F-665FF8AC21B0}"/>
-    <hyperlink ref="B94" r:id="rId67" xr:uid="{D28F01EF-DD36-4A79-8CB9-A7408133F926}"/>
-    <hyperlink ref="B95" r:id="rId68" xr:uid="{CBD12492-1ABB-4718-8F16-48DAFF5970D7}"/>
-    <hyperlink ref="B96" r:id="rId69" xr:uid="{2D5451B6-AA34-41DA-AAFB-DA5EBB7BFB34}"/>
-    <hyperlink ref="B97" r:id="rId70" xr:uid="{B6E4EA6D-9B6C-441B-A8A2-CA158C43FE76}"/>
-    <hyperlink ref="B98" r:id="rId71" xr:uid="{F19F2C60-4535-4231-8E55-D05817E4C139}"/>
-    <hyperlink ref="B99" r:id="rId72" xr:uid="{7BCFE097-9E02-4421-B453-D481BFF1D15F}"/>
-    <hyperlink ref="B100" r:id="rId73" xr:uid="{6615F85D-CD23-458B-B881-9F5467860D89}"/>
-    <hyperlink ref="B102" r:id="rId74" xr:uid="{F926ABA8-5A8F-46CB-A25A-FEDF3C4B49E9}"/>
-    <hyperlink ref="B103" r:id="rId75" xr:uid="{A9E636BF-6FB4-448F-81EB-A23BBD43DADC}"/>
-    <hyperlink ref="B104" r:id="rId76" xr:uid="{8223D37A-E348-4C1C-A3D3-90E6260D1F13}"/>
-    <hyperlink ref="B106" r:id="rId77" xr:uid="{4DAB9E56-84A1-471F-88B4-CAE564E89240}"/>
-    <hyperlink ref="B107" r:id="rId78" xr:uid="{CA08B2FB-E6A9-494F-9F69-8C32547DBBAD}"/>
-    <hyperlink ref="B108" r:id="rId79" xr:uid="{88CFB6EA-A942-49DF-A8C3-997A3359A1A4}"/>
-    <hyperlink ref="B109" r:id="rId80" xr:uid="{DD5DEE96-23E1-4D19-8E11-E60110696A05}"/>
-    <hyperlink ref="B112" r:id="rId81" xr:uid="{FB94DF08-EC18-4383-A985-425520F84659}"/>
-    <hyperlink ref="B113" r:id="rId82" xr:uid="{5FFCAB2A-DF67-4273-BB83-42718D2F722E}"/>
-    <hyperlink ref="B114" r:id="rId83" xr:uid="{D41AC6B9-0A37-44EF-A022-39DF12636823}"/>
-    <hyperlink ref="B115" r:id="rId84" xr:uid="{0F67069A-29F3-4028-B5F0-89C69DB1E009}"/>
-    <hyperlink ref="B116" r:id="rId85" xr:uid="{5A4FACBD-2B00-4387-9E9C-B35585E4C1C5}"/>
-    <hyperlink ref="B117" r:id="rId86" xr:uid="{CD7092F3-6261-48AD-B0FA-90221586FFBC}"/>
-    <hyperlink ref="B119" r:id="rId87" xr:uid="{4AA4C8D2-A8DA-45AF-A66C-E83FA918DB56}"/>
-    <hyperlink ref="B122" r:id="rId88" xr:uid="{9E7A9C74-1588-49BE-B1B5-3AF284CF12DA}"/>
-    <hyperlink ref="B123" r:id="rId89" xr:uid="{20685E0C-33BA-416D-873F-4FCB2AE7118B}"/>
-    <hyperlink ref="B124" r:id="rId90" xr:uid="{2F129F6F-C644-491A-AF40-4BC380EDDE5B}"/>
-    <hyperlink ref="B125" r:id="rId91" xr:uid="{ABF04FCD-0143-4ED7-A3A5-378194DA0652}"/>
-    <hyperlink ref="B126" r:id="rId92" xr:uid="{B9CDF478-6CA9-4C70-919D-272BB63D3D95}"/>
-    <hyperlink ref="B128" r:id="rId93" xr:uid="{AB2A82CE-778C-44D9-8C4C-68ED5AC18BB2}"/>
-    <hyperlink ref="B129" r:id="rId94" xr:uid="{D9B63067-04AB-4D1A-A79D-A84D8EBE3678}"/>
-    <hyperlink ref="B130" r:id="rId95" xr:uid="{3F602529-3E68-4689-B4B7-4D1E224C3426}"/>
-    <hyperlink ref="B131" r:id="rId96" xr:uid="{677800CB-E944-4EA2-BD0C-7FBF08AF638F}"/>
-    <hyperlink ref="B132" r:id="rId97" xr:uid="{46D3CAD0-311C-490F-A2F1-3A8EABE1F3D7}"/>
-    <hyperlink ref="B133" r:id="rId98" xr:uid="{E6838C8A-8FA2-43A8-992E-F4103C96FBAC}"/>
-    <hyperlink ref="B135" r:id="rId99" xr:uid="{7CB61DD4-8AC7-499A-A0BE-DB9FCF4D0592}"/>
-    <hyperlink ref="B136" r:id="rId100" xr:uid="{D9CB03D5-3686-442C-ACF5-B193209E5D81}"/>
-    <hyperlink ref="B137" r:id="rId101" xr:uid="{33F105D2-D779-4F8E-BE81-176BC3A4C5EF}"/>
-    <hyperlink ref="B142" r:id="rId102" xr:uid="{82446D98-CA37-4CDC-9B8E-7DCCA49CABD5}"/>
-    <hyperlink ref="B144" r:id="rId103" xr:uid="{AA44BF90-FE47-4AF8-8059-0A6598E75C83}"/>
-    <hyperlink ref="B147" r:id="rId104" xr:uid="{76E2A8F1-72C9-42A6-8BC8-38108BE118E9}"/>
-    <hyperlink ref="B149" r:id="rId105" xr:uid="{49DFCA2D-9377-4493-8931-F0B5DDAD7D6B}"/>
-    <hyperlink ref="B150" r:id="rId106" xr:uid="{103D4B0E-5B49-4CE1-9D7D-F67404FF26FB}"/>
-    <hyperlink ref="B152" r:id="rId107" xr:uid="{6EC2DF48-3605-4271-9671-5D05D13FCB08}"/>
-    <hyperlink ref="B153" r:id="rId108" xr:uid="{257FD368-8881-4305-AF2E-2E7D24C75683}"/>
-    <hyperlink ref="B154" r:id="rId109" xr:uid="{8129FCAE-A443-45D9-9DFF-D5A4A681ED7E}"/>
-    <hyperlink ref="B158" r:id="rId110" xr:uid="{4CDA3A7D-6B1E-4DD6-871E-7A16612477AE}"/>
-    <hyperlink ref="B159" r:id="rId111" xr:uid="{2FA76E6C-67F5-4C2A-92B9-CC0E4CFA1A6D}"/>
-    <hyperlink ref="B160" r:id="rId112" xr:uid="{AEACE583-AF51-45AB-A723-0EFA6589394A}"/>
-    <hyperlink ref="B161" r:id="rId113" xr:uid="{8BD177E3-216A-44B0-8311-7CFC452BD5CD}"/>
-    <hyperlink ref="B162" r:id="rId114" xr:uid="{928110A0-B879-4E8F-B408-C7849A0FE348}"/>
-    <hyperlink ref="B163" r:id="rId115" xr:uid="{14046852-0BB7-4125-90EA-28EAFFFCD2ED}"/>
-    <hyperlink ref="B164" r:id="rId116" xr:uid="{AE627CFB-09F1-4693-ACDA-8303B143D579}"/>
-    <hyperlink ref="B165" r:id="rId117" xr:uid="{E8423FEC-1488-40B4-9032-7B31EAFAD656}"/>
-    <hyperlink ref="B166" r:id="rId118" xr:uid="{97749151-F68D-431F-BF72-A52C8EB91B53}"/>
-    <hyperlink ref="B167" r:id="rId119" xr:uid="{71246596-ED82-4361-915D-C2B23AA129D7}"/>
-    <hyperlink ref="B169" r:id="rId120" xr:uid="{3AE660F5-089B-40D6-9A3C-B6B1861FB67F}"/>
-    <hyperlink ref="B171" r:id="rId121" xr:uid="{75E6EE40-887A-4812-8055-B8DB7478B2A7}"/>
-    <hyperlink ref="B172" r:id="rId122" xr:uid="{E3478E02-65D9-411F-BA75-CE8CEBBC828A}"/>
-    <hyperlink ref="B173" r:id="rId123" xr:uid="{64DA5C37-821B-44F2-B8CB-5E5EDDB6FAAB}"/>
-    <hyperlink ref="B175" r:id="rId124" xr:uid="{3986EEB5-F126-42F1-A1A8-6F683AA0F564}"/>
-    <hyperlink ref="B176" r:id="rId125" xr:uid="{F816A0F8-9F06-468D-A4A7-0A46D2D78827}"/>
-    <hyperlink ref="B177" r:id="rId126" xr:uid="{EB74B3FB-EC63-409D-9F39-389F5C2682FE}"/>
-    <hyperlink ref="B179" r:id="rId127" xr:uid="{71663150-B8FC-452F-BA6D-4A6A9F47F25F}"/>
-    <hyperlink ref="B180" r:id="rId128" xr:uid="{F3897E84-B2E4-4556-B188-5A076C2561DD}"/>
-    <hyperlink ref="B183" r:id="rId129" xr:uid="{5E40E090-0E1F-40AF-A2A9-5F1F234FFFB9}"/>
-    <hyperlink ref="B184" r:id="rId130" xr:uid="{D958013F-321B-4D5B-A24C-C333193B20F1}"/>
-    <hyperlink ref="B185" r:id="rId131" xr:uid="{7A77E3E8-B570-4D40-85E0-49DBC0A6FEFD}"/>
-    <hyperlink ref="B186" r:id="rId132" xr:uid="{B5A6D0BB-5AC0-4A81-A4E9-39F5FB6D8FFC}"/>
-    <hyperlink ref="B189" r:id="rId133" xr:uid="{E1069E5D-984B-421D-9A7F-E7C95D685D65}"/>
-    <hyperlink ref="B190" r:id="rId134" xr:uid="{0CDC9379-4303-44E5-A5CD-F446EEAEA8C5}"/>
-    <hyperlink ref="B191" r:id="rId135" xr:uid="{44891D86-5B34-4833-AB1F-E63431A42FA1}"/>
-    <hyperlink ref="B192" r:id="rId136" xr:uid="{D98FD578-FB9B-4A8F-9906-A9572867F80C}"/>
-    <hyperlink ref="B193" r:id="rId137" xr:uid="{5E5B4C45-ECC7-4A4B-8A6E-BFF28C98AEFA}"/>
-    <hyperlink ref="B194" r:id="rId138" xr:uid="{3E87ECB1-0B77-4E0B-9560-1460EC433888}"/>
-    <hyperlink ref="B195" r:id="rId139" xr:uid="{7C9D3D32-3458-40E6-89B6-318104A98324}"/>
-    <hyperlink ref="B196" r:id="rId140" xr:uid="{7520A767-2144-4539-A68B-2E0A508D3A43}"/>
-    <hyperlink ref="B197" r:id="rId141" xr:uid="{7C1C69B7-DA5B-47DB-AD80-4B60D6E9E33E}"/>
-    <hyperlink ref="B198" r:id="rId142" xr:uid="{D9F5D7C6-1A94-4D51-9F81-CDCA023DEACE}"/>
-    <hyperlink ref="B199" r:id="rId143" xr:uid="{E35CAED7-75CE-4139-AC4F-7F6F95D2E490}"/>
-    <hyperlink ref="B200" r:id="rId144" xr:uid="{D4E9439F-D6E9-44EF-B0AE-B120004AFF0A}"/>
-    <hyperlink ref="B201" r:id="rId145" xr:uid="{44A89A50-C07D-473B-B03E-EBC28ED63FC9}"/>
-    <hyperlink ref="B202" r:id="rId146" xr:uid="{177C2F46-C75E-4F8D-A6A2-6F1BB932751D}"/>
-    <hyperlink ref="B203" r:id="rId147" xr:uid="{F5EFBDB9-60AD-4D0E-8A6A-8E0A8F0A0C23}"/>
-    <hyperlink ref="B205" r:id="rId148" xr:uid="{7CE2D5BA-76E4-46AF-BC0A-3FAC2A8077BA}"/>
-    <hyperlink ref="B206" r:id="rId149" xr:uid="{AC40AF8E-0EAF-44D7-B9CF-75E9C72E65DD}"/>
-    <hyperlink ref="B208" r:id="rId150" xr:uid="{8FEA005D-957B-4D83-8F22-FFCCD9E0BF15}"/>
-    <hyperlink ref="B209" r:id="rId151" xr:uid="{51C0D049-E37B-4979-B7D7-4BE5E9EE1340}"/>
-    <hyperlink ref="B210" r:id="rId152" xr:uid="{FDA75FF0-A0EF-463F-A583-D91262ED5B01}"/>
-    <hyperlink ref="B211" r:id="rId153" xr:uid="{3244C81D-33D7-4398-BC2D-7DD0C91FFC66}"/>
-    <hyperlink ref="B212" r:id="rId154" xr:uid="{2C8A778E-CFC4-4543-ADF4-B91F27344114}"/>
-    <hyperlink ref="B215" r:id="rId155" xr:uid="{EED5890E-3B7D-41AA-B7D7-365BD323AF14}"/>
-    <hyperlink ref="B216" r:id="rId156" xr:uid="{55A7C955-45CC-4A55-ACF4-3206F66E41E2}"/>
-    <hyperlink ref="B218" r:id="rId157" xr:uid="{202C6CD5-821B-48CF-9EA0-D7AED1636046}"/>
-    <hyperlink ref="B220" r:id="rId158" xr:uid="{C468DA84-61EC-4E42-9FA4-043D2EB7570B}"/>
-    <hyperlink ref="B27" r:id="rId159" xr:uid="{8C9B2C49-ACEE-4996-8B59-E56A288A6FC7}"/>
-    <hyperlink ref="B222" r:id="rId160" xr:uid="{DF6655F4-A9F9-4691-98C3-A9DCD312CD57}"/>
-    <hyperlink ref="B181" r:id="rId161" xr:uid="{B6008CBC-A1A5-4F8C-97B3-820395B3A916}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B21" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B22" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B25" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B26" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B29" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B31" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B32" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B33" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B34" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B36" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B37" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B38" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B39" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B40" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B41" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B42" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B43" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B44" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B45" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B46" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B47" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B48" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B49" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B52" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B53" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B54" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B55" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B56" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B58" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B59" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B62" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B64" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B65" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B66" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B68" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B69" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B70" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B71" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B72" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B73" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B74" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B76" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B79" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B80" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B82" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B83" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B85" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B86" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B87" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B88" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B89" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B90" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B91" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B92" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B93" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B94" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B95" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B96" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B97" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B98" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B99" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B100" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B102" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B103" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B104" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B106" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B107" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B108" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B109" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B112" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B113" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B114" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B115" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B116" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B117" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B119" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B122" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B123" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B124" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B125" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B126" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B128" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B129" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B130" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B131" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B132" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B133" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B135" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B136" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B137" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B142" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B144" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B147" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B149" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B150" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B152" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B153" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B154" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B158" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B159" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B160" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B161" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B162" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B163" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B164" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B165" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B166" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B167" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="B169" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B171" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="B172" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="B173" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="B175" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="B176" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="B177" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="B179" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B180" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B183" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B184" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B185" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B186" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="B189" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="B190" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="B191" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="B192" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B193" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="B194" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="B195" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="B196" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="B197" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="B198" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="B199" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="B200" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="B201" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="B202" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="B203" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="B205" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="B206" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="B208" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="B209" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="B210" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="B211" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="B212" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="B215" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="B216" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="B218" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="B220" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="B27" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="B222" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="B181" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="B240" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="B245" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="B255" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="B271" r:id="rId165" display="mailto:siddisu@uic.edu" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId162"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId166"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new fall 2021 projects
</commit_message>
<xml_diff>
--- a/datasheets/All names.xlsx
+++ b/datasheets/All names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinho\Documents\UIUC\ARCHES\Github\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B01753A-D9BA-4844-8B63-8C88DD978829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B039516F-0BFA-48B6-8D4A-4736D97D03B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$C$354</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$C$357</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="577">
   <si>
     <t>Name</t>
   </si>
@@ -567,9 +567,6 @@
     <t>philli@illinois.edu</t>
   </si>
   <si>
-    <t>Helen Nguyen</t>
-  </si>
-  <si>
     <t>thn@illinois.edu</t>
   </si>
   <si>
@@ -1200,9 +1197,6 @@
     <t>Pavithra Rajeswaran</t>
   </si>
   <si>
-    <t>Pearl Richard H</t>
-  </si>
-  <si>
     <t>Richard.H.Pearl@osfhealthcare.org</t>
   </si>
   <si>
@@ -1269,9 +1263,6 @@
     <t>rayan.a.elkattah@osfhealthcare.org</t>
   </si>
   <si>
-    <t>chittaranjan.v.reddy@osfhealthcare.org</t>
-  </si>
-  <si>
     <t>Rhonda L. Johnson</t>
   </si>
   <si>
@@ -1293,6 +1284,9 @@
     <t>tapping@uic.edu</t>
   </si>
   <si>
+    <t>Rick Pearl</t>
+  </si>
+  <si>
     <t>Riley Frenette</t>
   </si>
   <si>
@@ -1368,6 +1362,9 @@
     <t>ryanf@uic.edu</t>
   </si>
   <si>
+    <t>Ryan Reich</t>
+  </si>
+  <si>
     <t>Sandhya Pruthi</t>
   </si>
   <si>
@@ -1734,13 +1731,34 @@
     <t>nhovakim@illinois.edu</t>
   </si>
   <si>
+    <t>https://publish.illinois.edu/timperman/people/aaron-t-timperman/</t>
+  </si>
+  <si>
+    <t>Faculty page</t>
+  </si>
+  <si>
+    <t>https://ise.illinois.edu/directory/profile/arwool</t>
+  </si>
+  <si>
+    <t>https://stat.illinois.edu/directory/profile/achronop</t>
+  </si>
+  <si>
+    <t>https://peoria.medicine.uic.edu/departments/hse-pathology/faculty/name/andrew-darr/</t>
+  </si>
+  <si>
+    <t>https://peoria.medicine.uic.edu/connections/name/andrew-lancia/</t>
+  </si>
+  <si>
+    <t>https://cs.illinois.edu/about/people/faculty/soc1024</t>
+  </si>
+  <si>
+    <t>https://ece.illinois.edu/about/directory/faculty/acsinger</t>
+  </si>
+  <si>
     <t>Pei-Hsuan Hsieh</t>
   </si>
   <si>
     <t>Joseph Irudayaraj</t>
-  </si>
-  <si>
-    <t>Ryan Riech</t>
   </si>
 </sst>
 </file>
@@ -2115,10 +2133,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C325"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2133,7 +2152,7 @@
     <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2143,8 +2162,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2154,8 +2176,11 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2166,7 +2191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2176,8 +2201,11 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2185,10 +2213,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2199,7 +2227,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2207,17 +2235,17 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2228,7 +2256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2238,8 +2266,11 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2250,7 +2281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -2259,7 +2290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2269,8 +2300,11 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2278,19 +2312,25 @@
       <c r="C14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2300,24 +2340,27 @@
       <c r="C16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2337,7 +2380,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2388,7 +2431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -2419,7 +2462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2439,7 +2482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2503,7 +2546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -2558,7 +2601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -2569,7 +2612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -2613,7 +2656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -2624,7 +2667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -2635,7 +2678,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -2646,7 +2689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>92</v>
       </c>
@@ -2679,7 +2722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -2723,16 +2766,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>107</v>
       </c>
@@ -2759,19 +2802,19 @@
         <v>111</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -2805,7 +2848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>118</v>
       </c>
@@ -2849,7 +2892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>126</v>
       </c>
@@ -2860,7 +2903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>128</v>
       </c>
@@ -2871,7 +2914,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>130</v>
       </c>
@@ -2904,7 +2947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>136</v>
       </c>
@@ -2920,13 +2963,13 @@
         <v>138</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>139</v>
       </c>
@@ -2977,7 +3020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>147</v>
       </c>
@@ -3017,7 +3060,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>153</v>
       </c>
@@ -3039,7 +3082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>157</v>
       </c>
@@ -3050,7 +3093,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>159</v>
       </c>
@@ -3072,7 +3115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>163</v>
       </c>
@@ -3105,7 +3148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>169</v>
       </c>
@@ -3162,21 +3205,21 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
+        <v>499</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="C98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>180</v>
       </c>
-      <c r="C98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="B99" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="C99" t="s">
         <v>7</v>
@@ -3184,10 +3227,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
+        <v>182</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>184</v>
       </c>
       <c r="C100" t="s">
         <v>10</v>
@@ -3195,10 +3238,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>10</v>
@@ -3206,10 +3249,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>185</v>
+      </c>
+      <c r="B102" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>187</v>
       </c>
       <c r="C102" t="s">
         <v>10</v>
@@ -3217,10 +3260,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>187</v>
+      </c>
+      <c r="B103" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="C103" t="s">
         <v>10</v>
@@ -3228,10 +3271,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>189</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="C104" t="s">
         <v>10</v>
@@ -3239,7 +3282,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" t="s">
@@ -3248,10 +3291,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>192</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>194</v>
       </c>
       <c r="C106" t="s">
         <v>10</v>
@@ -3259,10 +3302,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>194</v>
+      </c>
+      <c r="B107" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>196</v>
       </c>
       <c r="C107" t="s">
         <v>10</v>
@@ -3270,10 +3313,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
+        <v>196</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="C108" t="s">
         <v>10</v>
@@ -3281,10 +3324,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>198</v>
+      </c>
+      <c r="B109" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="C109" t="s">
         <v>10</v>
@@ -3292,7 +3335,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" t="s">
@@ -3301,74 +3344,74 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
+        <v>202</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="C112" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>204</v>
       </c>
-      <c r="C112" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+      <c r="B113" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>206</v>
       </c>
-      <c r="C113" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+      <c r="B114" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>208</v>
       </c>
-      <c r="C114" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="B115" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="C115" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>210</v>
       </c>
-      <c r="C115" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="B116" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>212</v>
       </c>
-      <c r="C116" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+      <c r="B117" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="C117" t="s">
         <v>7</v>
@@ -3376,36 +3419,36 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B118" s="3"/>
       <c r="C118" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>215</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C119" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="C119" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="B120" s="3"/>
       <c r="C120" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" t="s">
@@ -3414,10 +3457,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>219</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>221</v>
       </c>
       <c r="C122" t="s">
         <v>10</v>
@@ -3425,10 +3468,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>221</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>223</v>
       </c>
       <c r="C123" t="s">
         <v>10</v>
@@ -3436,10 +3479,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>223</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="C124" t="s">
         <v>27</v>
@@ -3447,10 +3490,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>225</v>
+      </c>
+      <c r="B125" s="4" t="s">
         <v>226</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>227</v>
       </c>
       <c r="C125" t="s">
         <v>10</v>
@@ -3458,52 +3501,52 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>227</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="C126" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>229</v>
-      </c>
-      <c r="C126" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>230</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
+        <v>230</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="C128" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>232</v>
       </c>
-      <c r="C128" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+      <c r="B129" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="C129" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>234</v>
       </c>
-      <c r="C129" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
+      <c r="B130" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="C130" t="s">
         <v>7</v>
@@ -3511,32 +3554,32 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
+        <v>236</v>
+      </c>
+      <c r="B131" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="B131" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="C131" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
+        <v>238</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="C132" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>240</v>
       </c>
-      <c r="C132" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
+      <c r="B133" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="C133" t="s">
         <v>7</v>
@@ -3544,19 +3587,19 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B134" s="3"/>
       <c r="C134" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
+        <v>243</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="C135" t="s">
         <v>7</v>
@@ -3564,10 +3607,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
+        <v>245</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="C136" t="s">
         <v>27</v>
@@ -3575,10 +3618,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C137" t="s">
         <v>10</v>
@@ -3586,66 +3629,66 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B138" s="3"/>
       <c r="C138" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B139" s="3"/>
       <c r="C139" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B140" s="3"/>
       <c r="C140" s="3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B141" s="3"/>
       <c r="C141" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
+        <v>252</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="C142" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="C142" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="B143" s="3"/>
       <c r="C143" s="3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>255</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="C144" t="s">
         <v>7</v>
@@ -3653,7 +3696,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B145" s="3"/>
       <c r="C145" t="s">
@@ -3662,7 +3705,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B146" s="3"/>
       <c r="C146" s="3" t="s">
@@ -3671,10 +3714,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
+        <v>259</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>260</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>261</v>
       </c>
       <c r="C147" t="s">
         <v>10</v>
@@ -3682,7 +3725,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B148" s="3"/>
       <c r="C148" s="3" t="s">
@@ -3691,10 +3734,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>261</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="C149" t="s">
         <v>10</v>
@@ -3702,10 +3745,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
+        <v>263</v>
+      </c>
+      <c r="B150" s="4" t="s">
         <v>264</v>
-      </c>
-      <c r="B150" s="4" t="s">
-        <v>265</v>
       </c>
       <c r="C150" s="9" t="s">
         <v>10</v>
@@ -3713,7 +3756,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B151" s="3"/>
       <c r="C151" t="s">
@@ -3722,10 +3765,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
+        <v>266</v>
+      </c>
+      <c r="B152" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>268</v>
       </c>
       <c r="C152" t="s">
         <v>37</v>
@@ -3733,10 +3776,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
+        <v>268</v>
+      </c>
+      <c r="B153" s="4" t="s">
         <v>269</v>
-      </c>
-      <c r="B153" s="4" t="s">
-        <v>270</v>
       </c>
       <c r="C153" t="s">
         <v>10</v>
@@ -3744,10 +3787,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
+        <v>270</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="C154" t="s">
         <v>10</v>
@@ -3755,7 +3798,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B155" s="3"/>
       <c r="C155" s="3" t="s">
@@ -3764,28 +3807,28 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B156" s="3"/>
       <c r="C156" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B157" s="3"/>
       <c r="C157" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>275</v>
+      </c>
+      <c r="B158" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>277</v>
       </c>
       <c r="C158" t="s">
         <v>10</v>
@@ -3793,10 +3836,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
+        <v>277</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="C159" t="s">
         <v>10</v>
@@ -3804,32 +3847,32 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>279</v>
+      </c>
+      <c r="B160" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="C160" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
         <v>281</v>
       </c>
-      <c r="C160" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+      <c r="B161" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="C161" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
         <v>283</v>
       </c>
-      <c r="C161" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
+      <c r="B162" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="C162" t="s">
         <v>7</v>
@@ -3837,10 +3880,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
+        <v>285</v>
+      </c>
+      <c r="B163" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>287</v>
       </c>
       <c r="C163" t="s">
         <v>10</v>
@@ -3848,21 +3891,21 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>287</v>
+      </c>
+      <c r="B164" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="C164" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
         <v>289</v>
       </c>
-      <c r="C164" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
+      <c r="B165" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>291</v>
       </c>
       <c r="C165" t="s">
         <v>7</v>
@@ -3870,29 +3913,29 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
+        <v>291</v>
+      </c>
+      <c r="B166" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="C166" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>293</v>
       </c>
-      <c r="C166" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
+      <c r="B167" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="C167" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="3" t="s">
         <v>295</v>
-      </c>
-      <c r="C167" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168" s="3" t="s">
-        <v>296</v>
       </c>
       <c r="B168" s="3"/>
       <c r="C168" s="3" t="s">
@@ -3901,41 +3944,41 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
+        <v>296</v>
+      </c>
+      <c r="B169" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="C169" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
         <v>298</v>
-      </c>
-      <c r="C169" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
-        <v>299</v>
       </c>
       <c r="B170" s="3"/>
       <c r="C170" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
+        <v>299</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="C171" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
         <v>301</v>
       </c>
-      <c r="C171" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
+      <c r="B172" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="C172" t="s">
         <v>7</v>
@@ -3943,10 +3986,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
+        <v>303</v>
+      </c>
+      <c r="B173" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="B173" s="4" t="s">
-        <v>305</v>
       </c>
       <c r="C173" t="s">
         <v>10</v>
@@ -3954,10 +3997,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="B174" s="3" t="s">
         <v>566</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>567</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>10</v>
@@ -3965,21 +4008,21 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
+        <v>305</v>
+      </c>
+      <c r="B175" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="C175" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
         <v>307</v>
       </c>
-      <c r="C175" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
+      <c r="B176" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>309</v>
       </c>
       <c r="C176" t="s">
         <v>7</v>
@@ -3987,10 +4030,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
+        <v>309</v>
+      </c>
+      <c r="B177" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="B177" s="4" t="s">
-        <v>311</v>
       </c>
       <c r="C177" t="s">
         <v>10</v>
@@ -3998,7 +4041,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B178" s="3"/>
       <c r="C178" t="s">
@@ -4007,21 +4050,21 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>312</v>
+      </c>
+      <c r="B179" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="C179" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
         <v>314</v>
       </c>
-      <c r="C179" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
+      <c r="B180" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="C180" t="s">
         <v>7</v>
@@ -4029,41 +4072,41 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
+        <v>316</v>
+      </c>
+      <c r="B181" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="B181" s="10" t="s">
+      <c r="C181" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="C181" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182" s="3" t="s">
-        <v>319</v>
       </c>
       <c r="B182" s="3"/>
       <c r="C182" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
+        <v>319</v>
+      </c>
+      <c r="B183" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="C183" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
         <v>321</v>
       </c>
-      <c r="C183" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
+      <c r="B184" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>323</v>
       </c>
       <c r="C184" t="s">
         <v>7</v>
@@ -4071,29 +4114,29 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>323</v>
+      </c>
+      <c r="B185" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="C185" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
         <v>325</v>
       </c>
-      <c r="C185" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
+      <c r="B186" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="C186" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="C186" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187" s="3" t="s">
-        <v>328</v>
       </c>
       <c r="B187" s="3"/>
       <c r="C187" s="3" t="s">
@@ -4102,10 +4145,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B188" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>330</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>10</v>
@@ -4113,10 +4156,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
+        <v>330</v>
+      </c>
+      <c r="B189" s="4" t="s">
         <v>331</v>
-      </c>
-      <c r="B189" s="4" t="s">
-        <v>332</v>
       </c>
       <c r="C189" t="s">
         <v>10</v>
@@ -4124,21 +4167,21 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
+        <v>332</v>
+      </c>
+      <c r="B190" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="C190" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
         <v>334</v>
       </c>
-      <c r="C190" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
+      <c r="B191" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>336</v>
       </c>
       <c r="C191" t="s">
         <v>7</v>
@@ -4146,10 +4189,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
+        <v>336</v>
+      </c>
+      <c r="B192" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="B192" s="4" t="s">
-        <v>338</v>
       </c>
       <c r="C192" t="s">
         <v>10</v>
@@ -4157,10 +4200,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
+        <v>338</v>
+      </c>
+      <c r="B193" s="4" t="s">
         <v>339</v>
-      </c>
-      <c r="B193" s="4" t="s">
-        <v>340</v>
       </c>
       <c r="C193" t="s">
         <v>10</v>
@@ -4168,21 +4211,21 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
+        <v>340</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="C194" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
+        <v>342</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="C195" t="s">
         <v>7</v>
@@ -4190,10 +4233,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
+        <v>344</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="C196" t="s">
         <v>27</v>
@@ -4201,43 +4244,43 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
+        <v>346</v>
+      </c>
+      <c r="B197" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>348</v>
       </c>
       <c r="C197" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
+        <v>348</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="C198" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
         <v>350</v>
       </c>
-      <c r="C198" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199" t="s">
+      <c r="B199" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B199" s="2" t="s">
+      <c r="C199" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
         <v>352</v>
       </c>
-      <c r="C199" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
+      <c r="B200" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="C200" t="s">
         <v>7</v>
@@ -4245,21 +4288,21 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>354</v>
+      </c>
+      <c r="B201" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="B201" s="4" t="s">
+      <c r="C201" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
         <v>356</v>
       </c>
-      <c r="C201" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
+      <c r="B202" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="B202" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="C202" t="s">
         <v>7</v>
@@ -4267,10 +4310,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
+        <v>358</v>
+      </c>
+      <c r="B203" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="B203" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="C203" t="s">
         <v>10</v>
@@ -4278,7 +4321,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B204" s="3"/>
       <c r="C204" t="s">
@@ -4287,39 +4330,39 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
+        <v>361</v>
+      </c>
+      <c r="B205" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="C205" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
         <v>363</v>
       </c>
-      <c r="C205" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
+      <c r="B206" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B206" s="2" t="s">
+      <c r="C206" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="3" t="s">
         <v>365</v>
-      </c>
-      <c r="C206" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A207" s="3" t="s">
-        <v>366</v>
       </c>
       <c r="B207" s="3"/>
       <c r="C207" s="3"/>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
+        <v>366</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>368</v>
       </c>
       <c r="C208" t="s">
         <v>7</v>
@@ -4327,10 +4370,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
+        <v>368</v>
+      </c>
+      <c r="B209" s="4" t="s">
         <v>369</v>
-      </c>
-      <c r="B209" s="4" t="s">
-        <v>370</v>
       </c>
       <c r="C209" t="s">
         <v>10</v>
@@ -4338,10 +4381,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
+        <v>370</v>
+      </c>
+      <c r="B210" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="B210" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="C210" t="s">
         <v>10</v>
@@ -4349,21 +4392,21 @@
     </row>
     <row r="211" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
+        <v>372</v>
+      </c>
+      <c r="B211" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="B211" s="5" t="s">
+      <c r="C211" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
         <v>374</v>
       </c>
-      <c r="C211" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A212" t="s">
+      <c r="B212" s="4" t="s">
         <v>375</v>
-      </c>
-      <c r="B212" s="4" t="s">
-        <v>376</v>
       </c>
       <c r="C212" t="s">
         <v>7</v>
@@ -4371,7 +4414,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B213" s="3"/>
       <c r="C213" s="3" t="s">
@@ -4380,19 +4423,19 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B214" s="3"/>
       <c r="C214" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
+        <v>378</v>
+      </c>
+      <c r="B215" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="C215" t="s">
         <v>7</v>
@@ -4400,10 +4443,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
+        <v>380</v>
+      </c>
+      <c r="B216" s="4" t="s">
         <v>381</v>
-      </c>
-      <c r="B216" s="4" t="s">
-        <v>382</v>
       </c>
       <c r="C216" t="s">
         <v>10</v>
@@ -4411,19 +4454,19 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B217" s="3"/>
       <c r="C217" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
+        <v>383</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="C218" t="s">
         <v>7</v>
@@ -4431,19 +4474,19 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B219" s="3"/>
       <c r="C219" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
+        <v>386</v>
+      </c>
+      <c r="B220" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="C220" t="s">
         <v>7</v>
@@ -4451,7 +4494,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B221" s="3"/>
       <c r="C221" t="s">
@@ -4460,10 +4503,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>390</v>
+        <v>414</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C222" t="s">
         <v>27</v>
@@ -4471,7 +4514,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>10</v>
@@ -4479,10 +4522,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B224" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C224" t="s">
         <v>10</v>
@@ -4490,7 +4533,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C225" t="s">
         <v>10</v>
@@ -4498,10 +4541,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B226" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C226" t="s">
         <v>10</v>
@@ -4509,10 +4552,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B227" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C227" t="s">
         <v>10</v>
@@ -4520,10 +4563,10 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B228" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C228" t="s">
         <v>10</v>
@@ -4531,7 +4574,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>10</v>
@@ -4539,7 +4582,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>10</v>
@@ -4547,7 +4590,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>10</v>
@@ -4555,10 +4598,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B232" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C232" t="s">
         <v>10</v>
@@ -4566,7 +4609,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>10</v>
@@ -4574,10 +4617,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B234" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C234" t="s">
         <v>10</v>
@@ -4585,10 +4628,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B235" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C235" t="s">
         <v>10</v>
@@ -4596,21 +4639,21 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B236" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C236" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>77</v>
+        <v>409</v>
       </c>
       <c r="B237" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C237" t="s">
         <v>7</v>
@@ -4618,7 +4661,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C238" t="s">
         <v>27</v>
@@ -4626,21 +4669,21 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
+        <v>412</v>
+      </c>
+      <c r="B239" t="s">
+        <v>413</v>
+      </c>
+      <c r="C239" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>414</v>
+      </c>
+      <c r="B240" t="s">
         <v>415</v>
-      </c>
-      <c r="B239" t="s">
-        <v>416</v>
-      </c>
-      <c r="C239" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A240" t="s">
-        <v>417</v>
-      </c>
-      <c r="B240" t="s">
-        <v>418</v>
       </c>
       <c r="C240" t="s">
         <v>7</v>
@@ -4648,43 +4691,43 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
+        <v>416</v>
+      </c>
+      <c r="B241" t="s">
+        <v>417</v>
+      </c>
+      <c r="C241" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>418</v>
+      </c>
+      <c r="B242" t="s">
         <v>415</v>
       </c>
-      <c r="B241" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C241" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A242" t="s">
+      <c r="C242" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
         <v>419</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B243" t="s">
         <v>420</v>
       </c>
-      <c r="C242" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A243" t="s">
+      <c r="C243" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
         <v>421</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B244" t="s">
         <v>422</v>
-      </c>
-      <c r="C243" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A244" t="s">
-        <v>423</v>
-      </c>
-      <c r="B244" t="s">
-        <v>424</v>
       </c>
       <c r="C244" t="s">
         <v>7</v>
@@ -4692,10 +4735,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C245" t="s">
         <v>10</v>
@@ -4703,29 +4746,29 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
+        <v>425</v>
+      </c>
+      <c r="B246" t="s">
+        <v>426</v>
+      </c>
+      <c r="C246" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
         <v>427</v>
       </c>
-      <c r="B246" t="s">
+      <c r="C247" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
         <v>428</v>
       </c>
-      <c r="C246" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A247" t="s">
+      <c r="B248" t="s">
         <v>429</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A248" t="s">
-        <v>430</v>
-      </c>
-      <c r="B248" t="s">
-        <v>431</v>
       </c>
       <c r="C248" t="s">
         <v>7</v>
@@ -4733,10 +4776,10 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B249" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C249" t="s">
         <v>10</v>
@@ -4744,10 +4787,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B250" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C250" t="s">
         <v>10</v>
@@ -4755,10 +4798,10 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B251" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C251" t="s">
         <v>10</v>
@@ -4766,10 +4809,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B252" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C252" t="s">
         <v>10</v>
@@ -4777,10 +4820,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B253" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C253" t="s">
         <v>10</v>
@@ -4788,10 +4831,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B254" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C254" t="s">
         <v>10</v>
@@ -4799,43 +4842,43 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C255" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>570</v>
+        <v>444</v>
       </c>
       <c r="B256" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C256" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
+        <v>445</v>
+      </c>
+      <c r="B257" t="s">
         <v>446</v>
       </c>
-      <c r="B257" t="s">
+      <c r="C257" t="s">
         <v>447</v>
-      </c>
-      <c r="C257" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
+        <v>448</v>
+      </c>
+      <c r="B258" t="s">
         <v>449</v>
-      </c>
-      <c r="B258" t="s">
-        <v>450</v>
       </c>
       <c r="C258" t="s">
         <v>10</v>
@@ -4843,10 +4886,10 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
+        <v>450</v>
+      </c>
+      <c r="B259" t="s">
         <v>451</v>
-      </c>
-      <c r="B259" t="s">
-        <v>452</v>
       </c>
       <c r="C259" t="s">
         <v>10</v>
@@ -4854,10 +4897,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
+        <v>452</v>
+      </c>
+      <c r="B260" t="s">
         <v>453</v>
-      </c>
-      <c r="B260" t="s">
-        <v>454</v>
       </c>
       <c r="C260" t="s">
         <v>10</v>
@@ -4865,7 +4908,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C261" t="s">
         <v>27</v>
@@ -4873,73 +4916,73 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
+        <v>455</v>
+      </c>
+      <c r="B262" t="s">
         <v>456</v>
-      </c>
-      <c r="B262" t="s">
-        <v>457</v>
       </c>
       <c r="C262" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
+        <v>457</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
         <v>458</v>
       </c>
-      <c r="C263" s="3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A264" t="s">
+      <c r="B264" t="s">
         <v>459</v>
       </c>
-      <c r="B264" t="s">
+      <c r="C264" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
         <v>460</v>
       </c>
-      <c r="C264" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A265" t="s">
+      <c r="B265" t="s">
         <v>461</v>
       </c>
-      <c r="B265" t="s">
+      <c r="C265" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
         <v>462</v>
       </c>
-      <c r="C265" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A266" t="s">
+      <c r="B266" t="s">
         <v>463</v>
       </c>
-      <c r="B266" t="s">
+      <c r="C266" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
         <v>464</v>
       </c>
-      <c r="C266" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A267" t="s">
+      <c r="B267" t="s">
         <v>465</v>
       </c>
-      <c r="B267" t="s">
+      <c r="C267" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
         <v>466</v>
       </c>
-      <c r="C267" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A268" t="s">
+      <c r="B268" t="s">
         <v>467</v>
-      </c>
-      <c r="B268" t="s">
-        <v>468</v>
       </c>
       <c r="C268" t="s">
         <v>7</v>
@@ -4947,10 +4990,10 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
+        <v>468</v>
+      </c>
+      <c r="B269" t="s">
         <v>469</v>
-      </c>
-      <c r="B269" t="s">
-        <v>470</v>
       </c>
       <c r="C269" t="s">
         <v>10</v>
@@ -4958,10 +5001,10 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
+        <v>470</v>
+      </c>
+      <c r="B270" t="s">
         <v>471</v>
-      </c>
-      <c r="B270" t="s">
-        <v>472</v>
       </c>
       <c r="C270" t="s">
         <v>10</v>
@@ -4969,21 +5012,21 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
+        <v>472</v>
+      </c>
+      <c r="B271" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="B271" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="C271" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
+        <v>474</v>
+      </c>
+      <c r="B272" s="2" t="s">
         <v>475</v>
-      </c>
-      <c r="B272" s="2" t="s">
-        <v>476</v>
       </c>
       <c r="C272" t="s">
         <v>7</v>
@@ -4991,26 +5034,26 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
+        <v>476</v>
+      </c>
+      <c r="C273" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
         <v>477</v>
       </c>
-      <c r="C273" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A274" t="s">
+      <c r="C274" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
         <v>478</v>
       </c>
-      <c r="C274" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A275" t="s">
+      <c r="B275" t="s">
         <v>479</v>
-      </c>
-      <c r="B275" t="s">
-        <v>480</v>
       </c>
       <c r="C275" t="s">
         <v>7</v>
@@ -5018,10 +5061,10 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
+        <v>480</v>
+      </c>
+      <c r="B276" t="s">
         <v>481</v>
-      </c>
-      <c r="B276" t="s">
-        <v>482</v>
       </c>
       <c r="C276" t="s">
         <v>10</v>
@@ -5029,40 +5072,40 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
+        <v>482</v>
+      </c>
+      <c r="B277" t="s">
         <v>483</v>
       </c>
-      <c r="B277" t="s">
+      <c r="C277" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
         <v>484</v>
       </c>
-      <c r="C277" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A278" t="s">
+      <c r="B278" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="B278" s="2" t="s">
+      <c r="C278" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
         <v>486</v>
       </c>
-      <c r="C278" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A279" t="s">
-        <v>487</v>
-      </c>
       <c r="C279" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
+        <v>487</v>
+      </c>
+      <c r="B280" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="B280" s="2" t="s">
-        <v>489</v>
       </c>
       <c r="C280" t="s">
         <v>10</v>
@@ -5070,21 +5113,21 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
+        <v>489</v>
+      </c>
+      <c r="B281" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="B281" s="2" t="s">
+      <c r="C281" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
         <v>491</v>
       </c>
-      <c r="C281" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A282" t="s">
+      <c r="B282" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="B282" s="2" t="s">
-        <v>493</v>
       </c>
       <c r="C282" t="s">
         <v>7</v>
@@ -5092,21 +5135,21 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
+        <v>493</v>
+      </c>
+      <c r="B283" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="B283" s="2" t="s">
+      <c r="C283" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
         <v>495</v>
       </c>
-      <c r="C283" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A284" t="s">
-        <v>496</v>
-      </c>
       <c r="B284" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C284" t="s">
         <v>7</v>
@@ -5114,21 +5157,21 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
+        <v>496</v>
+      </c>
+      <c r="B285" t="s">
+        <v>538</v>
+      </c>
+      <c r="C285" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
         <v>497</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B286" t="s">
         <v>539</v>
-      </c>
-      <c r="C285" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A286" t="s">
-        <v>498</v>
-      </c>
-      <c r="B286" t="s">
-        <v>540</v>
       </c>
       <c r="C286" t="s">
         <v>7</v>
@@ -5136,10 +5179,10 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B287" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C287" t="s">
         <v>27</v>
@@ -5147,10 +5190,10 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B288" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C288" t="s">
         <v>10</v>
@@ -5158,29 +5201,29 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
+        <v>500</v>
+      </c>
+      <c r="B289" t="s">
+        <v>541</v>
+      </c>
+      <c r="C289" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
         <v>501</v>
       </c>
-      <c r="B289" t="s">
-        <v>542</v>
-      </c>
-      <c r="C289" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A290" t="s">
-        <v>502</v>
-      </c>
       <c r="C290" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C291" t="s">
         <v>10</v>
@@ -5188,7 +5231,7 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C292" t="s">
         <v>27</v>
@@ -5196,7 +5239,7 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C293" t="s">
         <v>10</v>
@@ -5204,48 +5247,48 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C294" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
+        <v>506</v>
+      </c>
+      <c r="B295" t="s">
+        <v>543</v>
+      </c>
+      <c r="C295" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
         <v>507</v>
       </c>
-      <c r="B295" t="s">
+      <c r="B296" t="s">
         <v>544</v>
       </c>
-      <c r="C295" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A296" t="s">
+      <c r="C296" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
         <v>508</v>
       </c>
-      <c r="B296" t="s">
-        <v>545</v>
-      </c>
-      <c r="C296" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A297" t="s">
-        <v>509</v>
-      </c>
       <c r="C297" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B298" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C298" t="s">
         <v>10</v>
@@ -5253,26 +5296,26 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C299" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C300" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B301" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C301" t="s">
         <v>10</v>
@@ -5280,15 +5323,15 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C302" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C303" t="s">
         <v>7</v>
@@ -5296,23 +5339,23 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
+        <v>515</v>
+      </c>
+      <c r="C304" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
         <v>516</v>
-      </c>
-      <c r="C304" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A305" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C306" t="s">
         <v>10</v>
@@ -5320,7 +5363,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C307" t="s">
         <v>10</v>
@@ -5328,10 +5371,10 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B308" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C308" t="s">
         <v>10</v>
@@ -5339,7 +5382,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C309" t="s">
         <v>10</v>
@@ -5347,21 +5390,21 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
+        <v>521</v>
+      </c>
+      <c r="B310" t="s">
+        <v>549</v>
+      </c>
+      <c r="C310" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
         <v>522</v>
       </c>
-      <c r="B310" t="s">
+      <c r="B311" t="s">
         <v>550</v>
-      </c>
-      <c r="C310" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A311" t="s">
-        <v>523</v>
-      </c>
-      <c r="B311" t="s">
-        <v>551</v>
       </c>
       <c r="C311" t="s">
         <v>7</v>
@@ -5369,10 +5412,10 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B312" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C312" t="s">
         <v>10</v>
@@ -5380,10 +5423,10 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B313" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C313" t="s">
         <v>10</v>
@@ -5391,10 +5434,10 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B314" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C314" t="s">
         <v>10</v>
@@ -5402,7 +5445,7 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C315" t="s">
         <v>27</v>
@@ -5410,7 +5453,7 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C316" t="s">
         <v>10</v>
@@ -5418,10 +5461,10 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B317" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C317" t="s">
         <v>10</v>
@@ -5429,7 +5472,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C318" t="s">
         <v>10</v>
@@ -5437,10 +5480,10 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B319" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C319" t="s">
         <v>10</v>
@@ -5448,10 +5491,10 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B320" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C320" t="s">
         <v>27</v>
@@ -5459,7 +5502,7 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C321" t="s">
         <v>10</v>
@@ -5467,10 +5510,10 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B322" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C322" t="s">
         <v>10</v>
@@ -5478,18 +5521,18 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
+        <v>534</v>
+      </c>
+      <c r="B323" t="s">
+        <v>558</v>
+      </c>
+      <c r="C323" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
         <v>535</v>
-      </c>
-      <c r="B323" t="s">
-        <v>559</v>
-      </c>
-      <c r="C323" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A324" t="s">
-        <v>536</v>
       </c>
       <c r="C324" t="s">
         <v>7</v>
@@ -5497,17 +5540,67 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B325" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C325" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>536</v>
+      </c>
+      <c r="B326" t="s">
+        <v>559</v>
+      </c>
+      <c r="C326" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="328" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="329" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="332" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="333" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="334" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="335" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="336" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="337" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="338" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="339" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="340" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="341" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="342" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="343" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="344" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="345" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="346" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="347" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="348" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="349" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="350" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="351" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="352" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="353" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="354" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="355" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="356" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="357" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A1:C354" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C357" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="UIC"/>
+        <filter val="UICOMP"/>
+        <filter val="UIUC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="mailto:arwool@illinois.edu" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -5670,20 +5763,19 @@
     <hyperlink ref="B27" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
     <hyperlink ref="B222" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
     <hyperlink ref="B181" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="B241" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="B245" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="B255" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="B271" r:id="rId165" display="mailto:siddisu@uic.edu" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="B278" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="B272" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="B280" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="B281" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="B282" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="B283" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="B291" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="B306" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="B245" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="B255" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="B271" r:id="rId164" display="mailto:siddisu@uic.edu" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="B278" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="B272" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="B280" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="B281" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="B282" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="B283" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="B291" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="B306" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId174"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId173"/>
 </worksheet>
 </file>
</xml_diff>